<commit_message>
More translations, TODO: Repair Finish page - some languages do not work correctly
</commit_message>
<xml_diff>
--- a/models/Czech.xlsx
+++ b/models/Czech.xlsx
@@ -3708,13 +3708,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -3766,7 +3766,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3780,22 +3780,25 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -4187,43 +4190,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="59.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="41.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="7.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="9.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="15.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="15.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="15.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="47.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="11" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="11" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="11" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="59.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="41.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="7.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="9.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="15.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="15.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="11.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="15.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="47.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="13.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="12" width="20.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="12" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="12" width="18.576428571428572" customWidth="1" bestFit="1"/>
     <col min="21" max="21" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="11" width="25.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="11" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="11" width="17.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="11" width="18.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="11" width="14.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="27" max="27" style="11" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="12" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="12" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="12" width="17.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="12" width="18.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="12" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="12" width="20.862142857142857" customWidth="1" bestFit="1"/>
     <col min="28" max="28" style="6" width="81.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="29" max="29" style="6" width="81.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="30" max="30" style="6" width="81.14785714285713" customWidth="1" bestFit="1"/>
-    <col min="31" max="31" style="6" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="32" max="32" style="6" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="33" max="33" style="6" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="34" max="34" style="12" width="16.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="7" width="81.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="7" width="81.14785714285713" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="7" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="7" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="13" width="16.14785714285714" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>812</v>
       </c>
@@ -4323,11 +4326,11 @@
       <c r="AG1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1" t="s">
         <v>817</v>
       </c>
@@ -4412,7 +4415,7 @@
       <c r="AB2" s="1" t="s">
         <v>827</v>
       </c>
-      <c r="AC2" s="3"/>
+      <c r="AC2" s="9"/>
       <c r="AD2" s="1" t="s">
         <v>828</v>
       </c>
@@ -4425,11 +4428,11 @@
       <c r="AG2" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="AH2" s="9">
+      <c r="AH2" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>832</v>
       </c>
@@ -4527,11 +4530,11 @@
       <c r="AG3" s="1" t="s">
         <v>843</v>
       </c>
-      <c r="AH3" s="9">
+      <c r="AH3" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>844</v>
       </c>
@@ -4629,11 +4632,11 @@
       <c r="AG4" s="1" t="s">
         <v>856</v>
       </c>
-      <c r="AH4" s="9">
+      <c r="AH4" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>857</v>
       </c>
@@ -4733,11 +4736,11 @@
       <c r="AG5" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="AH5" s="9">
+      <c r="AH5" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>867</v>
       </c>
@@ -4835,11 +4838,11 @@
       <c r="AG6" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH6" s="9">
+      <c r="AH6" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>878</v>
       </c>
@@ -4937,11 +4940,11 @@
       <c r="AG7" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH7" s="9">
+      <c r="AH7" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1" t="s">
         <v>884</v>
       </c>
@@ -5041,11 +5044,11 @@
       <c r="AG8" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH8" s="9">
+      <c r="AH8" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1" t="s">
         <v>895</v>
       </c>
@@ -5143,11 +5146,11 @@
       <c r="AG9" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="AH9" s="9">
+      <c r="AH9" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1" t="s">
         <v>904</v>
       </c>
@@ -5245,11 +5248,11 @@
       <c r="AG10" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH10" s="9">
+      <c r="AH10" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1" t="s">
         <v>910</v>
       </c>
@@ -5349,11 +5352,11 @@
       <c r="AG11" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="AH11" s="9">
+      <c r="AH11" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1" t="s">
         <v>916</v>
       </c>
@@ -5451,11 +5454,11 @@
       <c r="AG12" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="AH12" s="9">
+      <c r="AH12" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1" t="s">
         <v>922</v>
       </c>
@@ -5555,11 +5558,11 @@
       <c r="AG13" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH13" s="9">
+      <c r="AH13" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1" t="s">
         <v>928</v>
       </c>
@@ -5657,11 +5660,11 @@
       <c r="AG14" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH14" s="9">
+      <c r="AH14" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1" t="s">
         <v>934</v>
       </c>
@@ -5759,11 +5762,11 @@
       <c r="AG15" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH15" s="9">
+      <c r="AH15" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="1" t="s">
         <v>941</v>
       </c>
@@ -5861,11 +5864,11 @@
       <c r="AG16" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH16" s="9">
+      <c r="AH16" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="1" t="s">
         <v>945</v>
       </c>
@@ -5961,11 +5964,11 @@
       <c r="AG17" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH17" s="9">
+      <c r="AH17" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="1" t="s">
         <v>952</v>
       </c>
@@ -6063,11 +6066,11 @@
       <c r="AG18" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="AH18" s="9">
+      <c r="AH18" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="1" t="s">
         <v>959</v>
       </c>
@@ -6165,11 +6168,11 @@
       <c r="AG19" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH19" s="9">
+      <c r="AH19" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="1" t="s">
         <v>965</v>
       </c>
@@ -6269,11 +6272,11 @@
       <c r="AG20" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH20" s="9">
+      <c r="AH20" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="1" t="s">
         <v>973</v>
       </c>
@@ -6371,11 +6374,11 @@
       <c r="AG21" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH21" s="10" t="s">
+      <c r="AH21" s="11" t="s">
         <v>978</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="1" t="s">
         <v>979</v>
       </c>
@@ -6460,7 +6463,7 @@
       <c r="AB22" s="1" t="s">
         <v>970</v>
       </c>
-      <c r="AC22" s="3"/>
+      <c r="AC22" s="9"/>
       <c r="AD22" s="1" t="s">
         <v>983</v>
       </c>
@@ -6473,11 +6476,11 @@
       <c r="AG22" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="AH22" s="9">
+      <c r="AH22" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="1" t="s">
         <v>985</v>
       </c>
@@ -6577,11 +6580,11 @@
       <c r="AG23" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH23" s="9">
+      <c r="AH23" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="1" t="s">
         <v>993</v>
       </c>
@@ -6681,11 +6684,11 @@
       <c r="AG24" s="1" t="s">
         <v>1000</v>
       </c>
-      <c r="AH24" s="9">
+      <c r="AH24" s="10">
         <f>FALSE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="1" t="s">
         <v>1001</v>
       </c>
@@ -6785,11 +6788,11 @@
       <c r="AG25" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="AH25" s="9">
+      <c r="AH25" s="10">
         <f>TRUE()</f>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
       <c r="A26" s="1" t="s">
         <v>1009</v>
       </c>
@@ -6889,7 +6892,7 @@
       <c r="AG26" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH26" s="9">
+      <c r="AH26" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -6991,7 +6994,7 @@
       <c r="AG27" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH27" s="9">
+      <c r="AH27" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -7095,7 +7098,7 @@
       <c r="AG28" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH28" s="9">
+      <c r="AH28" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -7195,7 +7198,7 @@
       <c r="AG29" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="AH29" s="9">
+      <c r="AH29" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -7284,7 +7287,7 @@
       <c r="AB30" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="AC30" s="3"/>
+      <c r="AC30" s="9"/>
       <c r="AD30" s="1" t="s">
         <v>1041</v>
       </c>
@@ -7297,7 +7300,7 @@
       <c r="AG30" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="AH30" s="9">
+      <c r="AH30" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -7386,7 +7389,7 @@
       <c r="AB31" s="1" t="s">
         <v>1040</v>
       </c>
-      <c r="AC31" s="3"/>
+      <c r="AC31" s="9"/>
       <c r="AD31" s="1" t="s">
         <v>1047</v>
       </c>
@@ -7399,7 +7402,7 @@
       <c r="AG31" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH31" s="9">
+      <c r="AH31" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -7501,7 +7504,7 @@
       <c r="AG32" s="1" t="s">
         <v>1056</v>
       </c>
-      <c r="AH32" s="9">
+      <c r="AH32" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -7605,7 +7608,7 @@
       <c r="AG33" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH33" s="9">
+      <c r="AH33" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -7707,7 +7710,7 @@
       <c r="AG34" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="AH34" s="9">
+      <c r="AH34" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -7811,7 +7814,7 @@
       <c r="AG35" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="AH35" s="9">
+      <c r="AH35" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -7903,7 +7906,7 @@
       <c r="AC36" s="1" t="s">
         <v>1082</v>
       </c>
-      <c r="AD36" s="3"/>
+      <c r="AD36" s="9"/>
       <c r="AE36" s="1" t="s">
         <v>841</v>
       </c>
@@ -7913,7 +7916,7 @@
       <c r="AG36" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH36" s="9">
+      <c r="AH36" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -8015,7 +8018,7 @@
       <c r="AG37" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH37" s="9">
+      <c r="AH37" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -8119,7 +8122,7 @@
       <c r="AG38" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH38" s="9">
+      <c r="AH38" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -8223,7 +8226,7 @@
       <c r="AG39" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH39" s="9">
+      <c r="AH39" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -8325,7 +8328,7 @@
       <c r="AG40" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="AH40" s="10" t="s">
+      <c r="AH40" s="11" t="s">
         <v>978</v>
       </c>
     </row>
@@ -8425,7 +8428,7 @@
       <c r="AG41" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH41" s="10" t="s">
+      <c r="AH41" s="11" t="s">
         <v>978</v>
       </c>
     </row>
@@ -8512,7 +8515,7 @@
       <c r="AB42" s="1" t="s">
         <v>1120</v>
       </c>
-      <c r="AC42" s="3"/>
+      <c r="AC42" s="9"/>
       <c r="AD42" s="1" t="s">
         <v>1121</v>
       </c>
@@ -8525,7 +8528,7 @@
       <c r="AG42" s="1" t="s">
         <v>1056</v>
       </c>
-      <c r="AH42" s="9">
+      <c r="AH42" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -8612,7 +8615,7 @@
       <c r="AB43" s="1" t="s">
         <v>1126</v>
       </c>
-      <c r="AC43" s="3"/>
+      <c r="AC43" s="9"/>
       <c r="AD43" s="1" t="s">
         <v>1127</v>
       </c>
@@ -8625,7 +8628,7 @@
       <c r="AG43" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="AH43" s="9">
+      <c r="AH43" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -8729,7 +8732,7 @@
       <c r="AG44" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="AH44" s="9">
+      <c r="AH44" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -8831,7 +8834,7 @@
       <c r="AG45" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH45" s="9">
+      <c r="AH45" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -8933,7 +8936,7 @@
       <c r="AG46" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH46" s="10" t="s">
+      <c r="AH46" s="11" t="s">
         <v>978</v>
       </c>
     </row>
@@ -9035,7 +9038,7 @@
       <c r="AG47" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH47" s="9">
+      <c r="AH47" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9135,7 +9138,7 @@
       <c r="AG48" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="AH48" s="9">
+      <c r="AH48" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -9222,7 +9225,7 @@
       <c r="AB49" s="1" t="s">
         <v>1160</v>
       </c>
-      <c r="AC49" s="3"/>
+      <c r="AC49" s="9"/>
       <c r="AD49" s="1" t="s">
         <v>1161</v>
       </c>
@@ -9235,7 +9238,7 @@
       <c r="AG49" s="1" t="s">
         <v>894</v>
       </c>
-      <c r="AH49" s="9">
+      <c r="AH49" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9337,7 +9340,7 @@
       <c r="AG50" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH50" s="9">
+      <c r="AH50" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9424,7 +9427,7 @@
       <c r="AB51" s="1" t="s">
         <v>1171</v>
       </c>
-      <c r="AC51" s="3"/>
+      <c r="AC51" s="9"/>
       <c r="AD51" s="1" t="s">
         <v>1172</v>
       </c>
@@ -9437,7 +9440,7 @@
       <c r="AG51" s="1" t="s">
         <v>831</v>
       </c>
-      <c r="AH51" s="9">
+      <c r="AH51" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9524,7 +9527,7 @@
       <c r="AB52" s="1" t="s">
         <v>1177</v>
       </c>
-      <c r="AC52" s="3"/>
+      <c r="AC52" s="9"/>
       <c r="AD52" s="1" t="s">
         <v>1178</v>
       </c>
@@ -9537,7 +9540,7 @@
       <c r="AG52" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="AH52" s="9">
+      <c r="AH52" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9626,7 +9629,7 @@
       <c r="AB53" s="1" t="s">
         <v>1182</v>
       </c>
-      <c r="AC53" s="3"/>
+      <c r="AC53" s="9"/>
       <c r="AD53" s="1" t="s">
         <v>1183</v>
       </c>
@@ -9639,7 +9642,7 @@
       <c r="AG53" s="1" t="s">
         <v>1056</v>
       </c>
-      <c r="AH53" s="9">
+      <c r="AH53" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9741,7 +9744,7 @@
       <c r="AG54" s="1" t="s">
         <v>903</v>
       </c>
-      <c r="AH54" s="9">
+      <c r="AH54" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9843,7 +9846,7 @@
       <c r="AG55" s="1" t="s">
         <v>915</v>
       </c>
-      <c r="AH55" s="9">
+      <c r="AH55" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -9945,7 +9948,7 @@
       <c r="AG56" s="1" t="s">
         <v>877</v>
       </c>
-      <c r="AH56" s="9">
+      <c r="AH56" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -10045,7 +10048,7 @@
       <c r="AG57" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH57" s="9">
+      <c r="AH57" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -10147,7 +10150,7 @@
       <c r="AG58" s="1" t="s">
         <v>1214</v>
       </c>
-      <c r="AH58" s="9">
+      <c r="AH58" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -10249,7 +10252,7 @@
       <c r="AG59" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH59" s="9">
+      <c r="AH59" s="10">
         <f>FALSE()</f>
       </c>
     </row>
@@ -10349,7 +10352,7 @@
       <c r="AG60" s="1" t="s">
         <v>927</v>
       </c>
-      <c r="AH60" s="9">
+      <c r="AH60" s="10">
         <f>TRUE()</f>
       </c>
     </row>
@@ -10373,28 +10376,28 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="13.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="19.862142857142857" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="8.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="16.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="38.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="23.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="41.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="6" width="60.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="6" width="28.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="6" width="35.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="6" width="60.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="6" width="27.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="6" width="47.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="6" width="70.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="6" width="37.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="6" width="45.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="6" width="63.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="6" width="26.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="6" width="38.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="6" width="47.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="38.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="8" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="41.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="60.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="35.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="60.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="47.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="70.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="7" width="37.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="45.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="63.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="7" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="7" width="38.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="7" width="47.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">

</xml_diff>